<commit_message>
Selected some demos for termination. Fixed others
the list is under ./CompuCell3D/core/Demos/demosFixing_README.md
</commit_message>
<xml_diff>
--- a/CompuCell3D/core/Demos/ProcessedDemos20-12-2018_16-45Darwin_failed_summary.xlsx
+++ b/CompuCell3D/core/Demos/ProcessedDemos20-12-2018_16-45Darwin_failed_summary.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>20-12-2018_16-45</t>
   </si>
@@ -36,78 +36,39 @@
     <t>[Return Code: 1]</t>
   </si>
   <si>
-    <t>Demos/BookChapterDemos_ComputationalMethodsInCellBiology/Angiogenesis/Angiogenesis.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] FileLockException: Timeout occured.</t>
   </si>
   <si>
-    <t>Demos/CompuCellPythonTutorial/clusterMitosisPeriodicBC/clusterMitosisPeriodicBC.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] AttributeError: VolumeParamSteppable instance has no attribute 'add_steering_panel'</t>
   </si>
   <si>
-    <t>Demos/CompuCellPythonTutorial/FiPyConcentrationTest/FiPyConcentrationTest.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] ImportError: No module named fipy</t>
   </si>
   <si>
-    <t>Demos/CompuCellPythonTutorial/GraphVTKVis/GraphVTKVis.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] ImportError: No module named networkx</t>
   </si>
   <si>
-    <t>Demos/CompuCellPythonTutorial/scientificPlots/scientificPlots.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] AttributeError: 'NoneType' object has no attribute 'size'</t>
   </si>
   <si>
-    <t>Demos/CompuCellPythonTutorial/vectorPlot/vectorPlot.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] AttributeError: VectorFieldPlotTestSteppable instance has no attribute 'add_steering_panel'</t>
   </si>
   <si>
-    <t>Demos/experimental/FiPyConcentrationTest/FiPyConcentrationTest.cc3d</t>
-  </si>
-  <si>
-    <t>Demos/experimental/GraphVTKVis/GraphVTKVis.cc3d</t>
-  </si>
-  <si>
     <t>Demos/Models/FitzHughNagumo_OpenCL/FitzHughNagumo_OpenCL.cc3d</t>
   </si>
   <si>
-    <t>Demos/optimization/optimization_demo/optimization_demo.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] GenericDrawer or basic simulation data is None. Could not output screenshots</t>
   </si>
   <si>
-    <t>Demos/PluginDemos/AdhesionFlexPython/AdhesionFlexPython.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] AttributeError: AdhesionMoleculesSteppables instance has no attribute 'add_steering_panel'</t>
   </si>
   <si>
-    <t>Demos/PluginDemos/elasticityTest_steering/elasticityTest_steering.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] AttributeError: ElasticitySteering instance has no attribute 'add_steering_panel'</t>
   </si>
   <si>
-    <t>Demos/PluginDemos/elongationTest_steering/elongationTest_steering.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] AttributeError: LengthConstraintSteering instance has no attribute 'add_steering_panel'</t>
   </si>
   <si>
-    <t>Demos/SteppableDemos/DiffusionSolverFE/diffusion_3D_scale_wall/diffusion_3D_scale_wall.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] FILE :/Users/m/CC3D_QT5_GIT/CompuCell3D/core/CompuCell3D/plugins/CellType/CellTypePlugin.cpp</t>
   </si>
   <si>
@@ -117,9 +78,6 @@
     <t>Demos/SteppableDemos/DiffusionSolverFE_OpenCL/DiffusionSolverFE_OpenCL_3D/DiffusionSolverFE_OpenCL_3D.cc3d</t>
   </si>
   <si>
-    <t>Demos/SteppableDemos/FlexibleDiffusionSolverFE/Steering/diffusion_steering.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] AttributeError: DiffusionSolverSteering instance has no attribute 'add_steering_panel'</t>
   </si>
   <si>
@@ -132,9 +90,6 @@
     <t>Mac OS 10.13.6 CC3D Version 3.7.9</t>
   </si>
   <si>
-    <t>[ERROR]  No chemical field has been loaded</t>
-  </si>
-  <si>
     <t>[ERROR]  deprecated/unsuported module (old diffusion solver)</t>
   </si>
   <si>
@@ -142,6 +97,48 @@
   </si>
   <si>
     <t>C:\Users\jferrari\Documents\CompuCell3D - dev stuff\code\CompuCell3D\core\</t>
+  </si>
+  <si>
+    <t>Demos/PluginDemos/AdhesionFlexPython/</t>
+  </si>
+  <si>
+    <t>Demos/SteppableDemos/FlexibleDiffusionSolverFE/Steering/</t>
+  </si>
+  <si>
+    <t>Demos/PluginDemos/elasticityTest_steering/</t>
+  </si>
+  <si>
+    <t>Demos/PluginDemos/elongationTest_steering/</t>
+  </si>
+  <si>
+    <t>Demos/CompuCellPythonTutorial/scientificPlots/</t>
+  </si>
+  <si>
+    <t>Demos/CompuCellPythonTutorial/vectorPlot/</t>
+  </si>
+  <si>
+    <t>Demos/CompuCellPythonTutorial/clusterMitosisPeriodicBC/</t>
+  </si>
+  <si>
+    <t>Demos/SteppableDemos/DiffusionSolverFE/diffusion_3D_scale_wall/</t>
+  </si>
+  <si>
+    <t>Demos/BookChapterDemos_ComputationalMethodsInCellBiology/Angiogenesis/</t>
+  </si>
+  <si>
+    <t>Demos/optimization/optimization_demo/</t>
+  </si>
+  <si>
+    <t>Demos/CompuCellPythonTutorial/FiPyConcentrationTest/</t>
+  </si>
+  <si>
+    <t>Demos/experimental/FiPyConcentrationTest/</t>
+  </si>
+  <si>
+    <t>Demos/CompuCellPythonTutorial/GraphVTKVis/</t>
+  </si>
+  <si>
+    <t>Demos/experimental/GraphVTKVis/</t>
   </si>
 </sst>
 </file>
@@ -305,7 +302,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -488,6 +485,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF5B5B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,7 +667,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -661,6 +676,12 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1024,7 +1045,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1059,7 +1080,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1067,21 +1088,21 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
+      <c r="A7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,10 +1110,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1100,10 +1121,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1111,10 +1132,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1122,10 +1143,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1133,10 +1154,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1144,10 +1165,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1155,21 +1176,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
+      <c r="A15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1177,10 +1198,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1188,43 +1209,43 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
+      <c r="A18" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="A19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>21</v>
+      <c r="A20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1232,10 +1253,10 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1243,10 +1264,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1254,10 +1275,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1265,10 +1286,10 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated readme and summary
</commit_message>
<xml_diff>
--- a/CompuCell3D/core/Demos/ProcessedDemos20-12-2018_16-45Darwin_failed_summary.xlsx
+++ b/CompuCell3D/core/Demos/ProcessedDemos20-12-2018_16-45Darwin_failed_summary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jferrari\Documents\CompuCell3D - dev stuff\code\CompuCell3D\core\Demos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\gitHub\CompuCell3D\CompuCell3D\core\Demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BE22EC-430C-479F-AF90-980F1F80732A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProcessedDemos20-12-2018_16-45D" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="40">
   <si>
     <t>20-12-2018_16-45</t>
   </si>
@@ -96,9 +97,6 @@
     <t>[ERROR] deprecated/unsuported module (old diffusion solver)</t>
   </si>
   <si>
-    <t>C:\Users\jferrari\Documents\CompuCell3D - dev stuff\code\CompuCell3D\core\</t>
-  </si>
-  <si>
     <t>Demos/PluginDemos/AdhesionFlexPython/</t>
   </si>
   <si>
@@ -139,12 +137,15 @@
   </si>
   <si>
     <t>Demos/experimental/GraphVTKVis/</t>
+  </si>
+  <si>
+    <t>C:\Users\julia\gitHub\CompuCell3D\CompuCell3D\core\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -302,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,6 +504,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -667,12 +674,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -682,6 +687,10 @@
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1041,254 +1050,254 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A21" sqref="A21:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="108.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.1328125" customWidth="1"/>
+    <col min="2" max="2" width="108.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="9" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="11" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="9" t="s">
+      <c r="C19" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="13" t="s">
+      <c r="C20" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="15" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed deprecated siffusion solver in demos
</commit_message>
<xml_diff>
--- a/CompuCell3D/core/Demos/ProcessedDemos20-12-2018_16-45Darwin_failed_summary.xlsx
+++ b/CompuCell3D/core/Demos/ProcessedDemos20-12-2018_16-45Darwin_failed_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\gitHub\CompuCell3D\CompuCell3D\core\Demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BE22EC-430C-479F-AF90-980F1F80732A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E36E73-9923-47B2-A5C7-5CE456736443}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>20-12-2018_16-45</t>
   </si>
@@ -55,9 +55,6 @@
     <t>[ERROR] AttributeError: VectorFieldPlotTestSteppable instance has no attribute 'add_steering_panel'</t>
   </si>
   <si>
-    <t>Demos/Models/FitzHughNagumo_OpenCL/FitzHughNagumo_OpenCL.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] GenericDrawer or basic simulation data is None. Could not output screenshots</t>
   </si>
   <si>
@@ -73,21 +70,9 @@
     <t>[ERROR] FILE :/Users/m/CC3D_QT5_GIT/CompuCell3D/core/CompuCell3D/plugins/CellType/CellTypePlugin.cpp</t>
   </si>
   <si>
-    <t>Demos/SteppableDemos/DiffusionSolverFE_OpenCL/DiffusionSolverFE_OpenCL/DiffusionSolverFE_OpenCL.cc3d</t>
-  </si>
-  <si>
-    <t>Demos/SteppableDemos/DiffusionSolverFE_OpenCL/DiffusionSolverFE_OpenCL_3D/DiffusionSolverFE_OpenCL_3D.cc3d</t>
-  </si>
-  <si>
     <t>[ERROR] AttributeError: DiffusionSolverSteering instance has no attribute 'add_steering_panel'</t>
   </si>
   <si>
-    <t>Demos/SteppableDemos/ReactionDiffusionSolverFE_OpenCL_Implicit/ReactionDiffusion_OpenCL_Implicit_3D/ReactionDiffusion_OpenCL_Implicit_3D.cc3d</t>
-  </si>
-  <si>
-    <t>Demos/SteppableDemos/ReactionDiffusionSolverFE_OpenCL_Implicit/SimpleDiffusion/SimpleDiffusion.cc3d</t>
-  </si>
-  <si>
     <t>Mac OS 10.13.6 CC3D Version 3.7.9</t>
   </si>
   <si>
@@ -140,6 +125,21 @@
   </si>
   <si>
     <t>C:\Users\julia\gitHub\CompuCell3D\CompuCell3D\core\</t>
+  </si>
+  <si>
+    <t>Demos/Models/FitzHughNagumo_OpenCL/</t>
+  </si>
+  <si>
+    <t>Demos/SteppableDemos/DiffusionSolverFE_OpenCL/DiffusionSolverFE_OpenCL/</t>
+  </si>
+  <si>
+    <t>Demos/SteppableDemos/DiffusionSolverFE_OpenCL/DiffusionSolverFE_OpenCL_3D</t>
+  </si>
+  <si>
+    <t>Demos/SteppableDemos/ReactionDiffusionSolverFE_OpenCL_Implicit/ReactionDiffusion_OpenCL_Implicit_3D/</t>
+  </si>
+  <si>
+    <t>Demos/SteppableDemos/ReactionDiffusionSolverFE_OpenCL_Implicit/SimpleDiffusion/</t>
   </si>
 </sst>
 </file>
@@ -485,12 +485,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF5B5B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -510,6 +504,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,10 +687,10 @@
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1054,7 +1054,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:C24"/>
+      <selection activeCell="A10" sqref="A10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1069,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -1089,62 +1089,62 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>24</v>
+      <c r="C10" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -1152,10 +1152,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -1163,10 +1163,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -1174,10 +1174,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -1185,20 +1185,20 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="A15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>10</v>
@@ -1218,91 +1218,91 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="7" t="s">
+      <c r="C23" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="15" t="s">
+      <c r="C24" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A6:C24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:C24">
     <sortCondition ref="A6:A24"/>
     <sortCondition ref="C6:C24"/>
   </sortState>

</xml_diff>